<commit_message>
Atualizacao DDD Turma 2
</commit_message>
<xml_diff>
--- a/Curso DDD/PlanoDeAula.xlsx
+++ b/Curso DDD/PlanoDeAula.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Aula DDD" sheetId="1" r:id="rId1"/>
     <sheet name="Plano de Aula Fundamentos em Ar" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Aula</t>
   </si>
@@ -83,15 +82,7 @@
     <t>Design Estratégico: Open Host Service/Published Language,Separate Ways,Anticorruption Layer</t>
   </si>
   <si>
-    <t>Explicação do conteúdo geral do curso
-Detalhando Ubiquitous Language
-Exercício em grupo para gerar um modelo inicial da solução do problema</t>
-  </si>
-  <si>
     <t>Building Blocks:Layered Architecture, Repositories</t>
-  </si>
-  <si>
-    <t>Não cheguei em fábricas e agregrações</t>
   </si>
   <si>
     <t>Building Blocks:Entities, Services, Value Objects, Agregates e Factories</t>
@@ -451,7 +442,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,19 +470,14 @@
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -499,7 +485,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -523,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>